<commit_message>
casos de pruebas mod
</commit_message>
<xml_diff>
--- a/test/Casos de Prueba.xlsx
+++ b/test/Casos de Prueba.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy\Documents\PythonDev\ProyectoVet2\projectcoder2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy\Documents\PythonDev\ProyectoVet2\projectcoder2\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AE6866-913A-4C9E-9C1F-FDF736BD8A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9039BF9-0D28-4328-B0EA-423EB652733C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -68,169 +68,6 @@
   </si>
   <si>
     <t>Media</t>
-  </si>
-  <si>
-    <t>Verificar Botón Info</t>
-  </si>
-  <si>
-    <t>Baja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Abrir la app
-2. Seleccionar la pestaña Prácticas
-3. Seleccionar una práctica (Ej, ""Camino"")
-4. Seleccionar una lección
-5. Seleccionar uno de los pasos de la lección
-6. Dar tap en ""Empezar""  
-7. Dar tap en "( i )" </t>
-  </si>
-  <si>
-    <t>Se muestra pantalla con la descripción de la meditación que contiene lo siguiente:
-Botón Cerrar
-Título de la meditación
-Texto descriptivo
-Autor/Narrador
-Biografía del Autor</t>
-  </si>
-  <si>
-    <t>.... IDEM para cada interacción posible.</t>
-  </si>
-  <si>
-    <t>Verificar Botón/Gesto Atrás del dispositivo</t>
-  </si>
-  <si>
-    <t>1. Abrir la app
-2. Seleccionar la pestaña Prácticas
-3. Seleccionar una práctica (Ej, "Camino")
-4. Seleccionar una lección
-5. Seleccionar uno de los pasos de la lección
-6. Dar tap en "Empezar"  
-7. Dar tap en Botón atrás / Hacer Gesto Atrás</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">7. Se muestra un modal de confirmación con las siguientes características:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Título: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Confirmación
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Mensaje: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">¿Está seguro de que desea cerrar la meditación?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Link:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> No
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Link:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Sí
-8. Se cierra el Modal y se mantiene en la pantalla de la meditación en el mismo estado (en reproducción o en pausa).
-9. Se cierra la meditación y se muestra la pantalla de el paso seleccionado con la lista de lecciones del día.</t>
-    </r>
-  </si>
-  <si>
-    <t>Verificar Reproducción en segundo plano - Reproducción en curso</t>
-  </si>
-  <si>
-    <t>1. Abrir la app
-2. Seleccionar la pestaña Prácticas
-3. Seleccionar una práctica (Ej, "Camino")
-4. Seleccionar una lección
-5. Seleccionar uno de los pasos de la lección
-6. Dar tap en "Empezar"  
-7. Salir de la app (enviar a segundo plano)
-8. Volver a abrir la app</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">7. Se detiene la reproducción </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">(depende de la definición que se adopte, por ejemplo Youtube gratis la detiene, Youtube Premium permite escuchar en segundo plano).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>8. Se retoma la reproducción el el mismo momento que estaba al salir.</t>
-    </r>
   </si>
   <si>
     <t>Nombre del Tester</t>
@@ -419,7 +256,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -476,18 +313,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
@@ -535,6 +360,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -573,9 +406,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -614,38 +447,41 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -906,7 +742,7 @@
   </sheetPr>
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B11:B14"/>
     </sheetView>
   </sheetViews>
@@ -955,13 +791,13 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1040,25 +876,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>32</v>
+        <v>20</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -1085,25 +921,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -1130,25 +966,25 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -1204,7 +1040,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="5" t="s">
@@ -1212,13 +1048,13 @@
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="5" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -1245,21 +1081,21 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>45</v>
+        <v>36</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -1286,7 +1122,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="5" t="s">
@@ -1294,13 +1130,13 @@
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -1324,7 +1160,7 @@
     </row>
     <row r="11" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
-      <c r="B11" s="5"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1353,7 +1189,7 @@
     </row>
     <row r="12" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
-      <c r="B12" s="5"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1382,7 +1218,7 @@
     </row>
     <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
-      <c r="B13" s="5"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1411,7 +1247,7 @@
     </row>
     <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -2589,7 +2425,7 @@
   <dimension ref="A1:AA53"/>
   <sheetViews>
     <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I6" sqref="B6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2637,13 +2473,13 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -2722,25 +2558,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>33</v>
+        <v>43</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -2766,11 +2602,11 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>27</v>
+      <c r="B5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>12</v>
@@ -2778,14 +2614,14 @@
       <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>57</v>
+      <c r="F5" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -2811,24 +2647,12 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -2850,11 +2674,9 @@
       <c r="Z6" s="7"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
-      <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B7" s="5"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -2885,20 +2707,12 @@
       <c r="A8" s="5">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B8" s="5"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="D8" s="5"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -2920,24 +2734,16 @@
       <c r="Z8" s="7"/>
       <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="1:27" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B9" s="5"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -4254,7 +4060,7 @@
   </sheetPr>
   <dimension ref="A1:AB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -4274,14 +4080,14 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -4306,12 +4112,12 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -4375,7 +4181,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>3</v>
@@ -4392,7 +4198,7 @@
       <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="24"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="4"/>
@@ -4416,14 +4222,14 @@
       <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>62</v>
+      <c r="B5" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>63</v>
+      <c r="D5" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>12</v>
@@ -4431,21 +4237,21 @@
       <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>61</v>
+      <c r="G5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="21"/>
+      <c r="O5" s="18"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
@@ -4464,14 +4270,14 @@
       <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>64</v>
+      <c r="B6" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="21" t="s">
-        <v>63</v>
+      <c r="D6" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>12</v>
@@ -4479,14 +4285,14 @@
       <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>30</v>
+      <c r="G6" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>33</v>
+        <v>54</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -4510,7 +4316,7 @@
     </row>
     <row r="7" spans="1:28" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
-      <c r="B7" s="21"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -5973,7 +5779,7 @@
     <col min="9" max="9" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5984,7 +5790,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -6001,7 +5807,7 @@
       <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="24"/>
+      <c r="J1" s="20"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -6010,14 +5816,14 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>66</v>
+      <c r="B2" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>63</v>
+      <c r="D2" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>12</v>
@@ -6025,14 +5831,14 @@
       <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>61</v>
+      <c r="G2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -6043,14 +5849,14 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>69</v>
+      <c r="B3" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>63</v>
+      <c r="D3" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>12</v>
@@ -6058,14 +5864,14 @@
       <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="21" t="s">
-        <v>33</v>
+      <c r="G3" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -6076,14 +5882,14 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>63</v>
+      <c r="B4" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>12</v>
@@ -6091,14 +5897,14 @@
       <c r="F4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>37</v>
+      <c r="G4" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -6136,7 +5942,7 @@
       <c r="M6" s="7"/>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="25"/>
+      <c r="C21" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>